<commit_message>
more papers and more reviews
</commit_message>
<xml_diff>
--- a/literature review/lit review.xlsx
+++ b/literature review/lit review.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="128">
   <si>
     <t>INDEX</t>
   </si>
@@ -43,7 +43,7 @@
     <t>SIGNATURE DIAGRAM</t>
   </si>
   <si>
-    <t>SENSORS</t>
+    <t>SENSORS/ HW</t>
   </si>
   <si>
     <t>TECH STACK</t>
@@ -298,13 +298,100 @@
     <t>009</t>
   </si>
   <si>
+    <t>Maciej M. Nowak, Katarzyna Dziȩob, Łukasz Ludwisiak, Julian Chmiel</t>
+  </si>
+  <si>
+    <t>Mobile GIS Applications for Environmental Field Surveys: A State of the Art</t>
+  </si>
+  <si>
+    <t>Mobile GIS applications exist but are underutilized and rarely documented in research methodology.No comprehensive review of mobile GIS applications for environmental field surveys exists</t>
+  </si>
+  <si>
+    <t>Provides a global review of mobile GIS applications for environmental fieldwork.Analyzes the capabilities of different mobile GIS tools like ArcGIS Collector, QField, Mapit Spatial, etc.Presents real-world case studies, including biodiversity mapping at a limestone mining site in Poland.Highlights the advantages of mobile GIS for field data collection compared to traditional methods</t>
+  </si>
+  <si>
+    <t>Review existing mobile GIS applications for environmental field surveys.</t>
+  </si>
+  <si>
+    <t>More widespread adoption of mobile GIS in research.Better documentation of GIS tools in academic papers.Integration with emerging technologies like UAVs (drones) for spatial mapping.</t>
+  </si>
+  <si>
     <t>010</t>
   </si>
   <si>
+    <t>Bernard Akindade Adaramola,Ayodeji Olalekan Salau , Favour Oluwatobi Adetunji , Olatomide Gbenga Fadodun , Adebayo Tunbosun Ogundipe</t>
+  </si>
+  <si>
+    <t>Development and Performance analysis of a GPS GSM Guided System for Vehicle Tracking</t>
+  </si>
+  <si>
+    <t>preventing car theft by creating an app that sends the car coordinates to the owner</t>
+  </si>
+  <si>
+    <t>created a fully functional app that sends an sms notification when recieving a message from the user and sends coordinates to authorities/user when theft is detected</t>
+  </si>
+  <si>
+    <t>to create an app that prevents theft and sends an sms to the users phone upon detection of theft (detected with a vibration detection module). the app will use gps and gms modules to send the coordinates.</t>
+  </si>
+  <si>
+    <t>NEO 6M GPS Module,  Piezoelectric Transducer, LM2940CT Voltage Regulator , MCP 602 Op Amp, arduino uno,  SIM 800l Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Proteus Software to test and model the circuit.</t>
+  </si>
+  <si>
+    <t>compared battery life, time to first fix (TTFF) (time to connect the module to the satellites), and accuracy of coordinates of the gps module.</t>
+  </si>
+  <si>
+    <t>the app was created and tested.</t>
+  </si>
+  <si>
     <t>011</t>
   </si>
   <si>
+    <t>Ugwu Nnaemeka Virginus1, Okafor, Loveth Ijeoma2, Ikechukwu Onyekachukwu3, Agbo, Jonathan Chukwunwike4, Uzoigwe Charles Ikechukwu5, Anyaorah Chukwuka Charles6, Udechukwu Precious Emeka7, Jonah Jane8, Obi Adaobi Maria9</t>
+  </si>
+  <si>
+    <t>Design and Implementation Vehicle Tracking System Using GSM and GPS</t>
+  </si>
+  <si>
+    <t>This paper presents a Vehicle Theft Alert and area ID arrangement utilizing GSM and GPS innovations.</t>
+  </si>
+  <si>
+    <t>a finished framework which sends an sms message to the authorities and user when the car starts and the mystery confirmation button isnt clicked within 40 seconds</t>
+  </si>
+  <si>
+    <t>. The point is to plan a framework that can trigger a SMS ready capacity that can make mindfulness for vehicle proprietors to assist them with checkmating unapproved faculty exercises on the vehicle and an area ID highlight utilizing GSM and GPS is additionally accessible to distinguish unapproved drivers and tos recover lost or taken vehicles.</t>
+  </si>
+  <si>
+    <t>Gsm module, GPS module</t>
+  </si>
+  <si>
+    <t>JAVA programming language, while PHP and MySQL were utilized for the web application capacities.</t>
+  </si>
+  <si>
     <t>012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rezowana Akter, Md Jahid Hasan Khandaker,Shakil Ahmed,Muhtasim Munem Mugdho,A K M Bahalul Haque </t>
+  </si>
+  <si>
+    <t>RFID based Smart Transportation System with Android Application</t>
+  </si>
+  <si>
+    <t>introducing a smart transportation system for public buses</t>
+  </si>
+  <si>
+    <t>2 applications, A user application has been developed which provides real-time information (bus location and fare) to the passenger that ensures an efficient public transportation system. and a driver application to keep count of passengers.</t>
+  </si>
+  <si>
+    <t>The main of this research work is to offer an effortless transportation facility by minimizing the problems faced by passengers, drivers and the concerned authorities with the help of a handy android application.</t>
+  </si>
+  <si>
+    <t>RFID, GPS module</t>
+  </si>
+  <si>
+    <t>firebase, and google maps</t>
   </si>
   <si>
     <t>013</t>
@@ -433,7 +520,7 @@
     <xdr:ext cx="3924300" cy="2514600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.jpg"/>
+        <xdr:cNvPr id="0" name="image8.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -461,7 +548,7 @@
     <xdr:ext cx="676275" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.jpg"/>
+        <xdr:cNvPr id="0" name="image9.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -489,7 +576,7 @@
     <xdr:ext cx="3924300" cy="2438400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.jpg"/>
+        <xdr:cNvPr id="0" name="image5.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -517,7 +604,7 @@
     <xdr:ext cx="295275" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.jpg"/>
+        <xdr:cNvPr id="0" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -545,7 +632,7 @@
     <xdr:ext cx="3829050" cy="1704975"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPr id="0" name="image3.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -573,7 +660,7 @@
     <xdr:ext cx="152400" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.jpg"/>
+        <xdr:cNvPr id="0" name="image10.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -601,11 +688,95 @@
     <xdr:ext cx="428625" cy="200025"/>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image7.jpg"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="419100" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image4.jpg"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="714375" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="0" name="image6.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="323850" cy="200025"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image2.jpg"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1284,85 +1455,213 @@
       <c r="A10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="B10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2020.0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
+      <c r="O10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="P10" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="D11" s="4">
+        <v>2020.0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="K11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
+      <c r="P11" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="D12" s="4">
+        <v>2020.0</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="K12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
+      <c r="P12" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="D13" s="4">
+        <v>2020.0</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="K13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1382,7 +1681,7 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1402,7 +1701,7 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1422,7 +1721,7 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1442,7 +1741,7 @@
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1462,7 +1761,7 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1482,7 +1781,7 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1502,7 +1801,7 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1522,7 +1821,7 @@
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1542,7 +1841,7 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1562,7 +1861,7 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>

</xml_diff>